<commit_message>
00 - 04 fig 1 updates
</commit_message>
<xml_diff>
--- a/cropped_and_labeled_image_data/2000_cropped_and_labeled_figs.xlsx
+++ b/cropped_and_labeled_image_data/2000_cropped_and_labeled_figs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1553,6 +1553,265 @@
         <v>1</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Bacharach et al._2000_ASQ_Boundary Management Tactics and Logics of Action.pdf</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>F1_P15_Bacharach et al._2000_ASQ_Boundary Management Tactics and Logics of Action.png</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E31" t="n">
+        <v>16</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>final_figures/2000/F1_P15_Bacharach et al._2000_ASQ_Boundary Management Tactics and Logics of Action.png</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>2x2 matrix</t>
+        </is>
+      </c>
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Maznevski &amp; Chudoba_2000_OrgSci_Bridging Qualitative and Quantitative Methods.pdf</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>F1_P14_Maznevski &amp; Chudoba_2000_OrgSci_Bridging Qualitative and Quantitative Methods.png</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E32" t="n">
+        <v>15</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>final_figures/2000/F1_P14_Maznevski &amp; Chudoba_2000_OrgSci_Bridging Qualitative and Quantitative Methods.png</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>process diagram</t>
+        </is>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Maznevski &amp; Chudoba_2000_OrgSci_Bridging Space over Time.pdf</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>F1_P15_Maznevski &amp; Chudoba_2000_OrgSci_Bridging Space over Time.png</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E33" t="n">
+        <v>16</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>final_figures/2000/F1_P15_Maznevski &amp; Chudoba_2000_OrgSci_Bridging Space over Time.png</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>process diagram</t>
+        </is>
+      </c>
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Orlikowski_2000_OrgSci_Using Technology and Constituting Structures.pdf</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>F1_P7_Orlikowski_2000_OrgSci_Using Technology and Constituting Structures.png</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E34" t="n">
+        <v>8</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>final_figures/2000/F1_P7_Orlikowski_2000_OrgSci_Using Technology and Constituting Structures.png</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>none selected</t>
+        </is>
+      </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Pratt_2000_ASQ_The Good, the Bad and the Ambivalent.pdf</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>F1_P21_Pratt_2000_ASQ_The Good, the Bad and the Ambivalent.png</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E35" t="n">
+        <v>22</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>final_figures/2000/F1_P21_Pratt_2000_ASQ_The Good, the Bad and the Ambivalent.png</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>conceptual diagram</t>
+        </is>
+      </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Shane_2000_OrgSci_Prior Knowledge and the Discovery of Entrepreneurial Opportunities.pdf</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>F1_P6_Shane_2000_OrgSci_Prior Knowledge and the Discovery of Entrepreneurial Opportunities.png</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E36" t="n">
+        <v>7</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>final_figures/2000/F1_P6_Shane_2000_OrgSci_Prior Knowledge and the Discovery of Entrepreneurial Opportunities.png</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>conceptual diagram</t>
+        </is>
+      </c>
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Voss et al._2000_OrgSci_Linking Organizational Values to Relationships with External Constituents_Quant.pdf</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>F1_P5_Voss et al._2000_OrgSci_Linking Organizational Values to Relationships with External Constituents_Quant.png</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E37" t="n">
+        <v>6</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>final_figures/2000/F1_P5_Voss et al._2000_OrgSci_Linking Organizational Values to Relationships with External Constituents_Quant.png</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>conceptual diagram</t>
+        </is>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
diagram labeling thru 2016
</commit_message>
<xml_diff>
--- a/cropped_and_labeled_image_data/2000_cropped_and_labeled_figs.xlsx
+++ b/cropped_and_labeled_image_data/2000_cropped_and_labeled_figs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,11 +474,6 @@
           <t>subcategory</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>is_viewed</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -513,9 +508,6 @@
           <t>2x2 matrix</t>
         </is>
       </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -550,9 +542,6 @@
           <t>process diagram</t>
         </is>
       </c>
-      <c r="I3" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -587,9 +576,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -624,9 +610,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -661,9 +644,6 @@
           <t>other</t>
         </is>
       </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -698,9 +678,6 @@
           <t>organizational chart</t>
         </is>
       </c>
-      <c r="I7" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -735,9 +712,6 @@
           <t>cycle</t>
         </is>
       </c>
-      <c r="I8" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -772,9 +746,6 @@
           <t>cycle</t>
         </is>
       </c>
-      <c r="I9" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -809,9 +780,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I10" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -846,9 +814,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I11" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -880,11 +845,8 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>line graph</t>
-        </is>
-      </c>
-      <c r="I12" t="b">
-        <v>1</v>
+          <t>line graph(s)</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -920,9 +882,6 @@
           <t>table</t>
         </is>
       </c>
-      <c r="I13" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -957,9 +916,6 @@
           <t>other</t>
         </is>
       </c>
-      <c r="I14" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -991,11 +947,8 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>line graph</t>
-        </is>
-      </c>
-      <c r="I15" t="b">
-        <v>1</v>
+          <t>line graph(s)</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -1028,11 +981,8 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>line graph</t>
-        </is>
-      </c>
-      <c r="I16" t="b">
-        <v>1</v>
+          <t>line graph(s)</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -1065,11 +1015,8 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>line graph</t>
-        </is>
-      </c>
-      <c r="I17" t="b">
-        <v>1</v>
+          <t>line graph(s)</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -1102,11 +1049,8 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>line graph</t>
-        </is>
-      </c>
-      <c r="I18" t="b">
-        <v>1</v>
+          <t>line graph(s)</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1142,9 +1086,6 @@
           <t>process diagram</t>
         </is>
       </c>
-      <c r="I19" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1179,9 +1120,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I20" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1216,9 +1154,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I21" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1253,9 +1188,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I22" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1287,11 +1219,8 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>drawing</t>
-        </is>
-      </c>
-      <c r="I23" t="b">
-        <v>1</v>
+          <t>drawing(s)</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1327,9 +1256,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I24" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1364,9 +1290,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I25" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1401,9 +1324,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I26" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1438,9 +1358,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I27" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1475,9 +1392,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I28" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1512,9 +1426,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I29" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1549,9 +1460,6 @@
           <t>timeline</t>
         </is>
       </c>
-      <c r="I30" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1586,9 +1494,6 @@
           <t>2x2 matrix</t>
         </is>
       </c>
-      <c r="I31" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1623,9 +1528,6 @@
           <t>process diagram</t>
         </is>
       </c>
-      <c r="I32" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1660,9 +1562,6 @@
           <t>process diagram</t>
         </is>
       </c>
-      <c r="I33" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1697,9 +1596,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I34" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1734,9 +1630,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I35" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1771,9 +1664,6 @@
           <t>conceptual diagram</t>
         </is>
       </c>
-      <c r="I36" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1807,9 +1697,6 @@
         <is>
           <t>conceptual diagram</t>
         </is>
-      </c>
-      <c r="I37" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>